<commit_message>
New data elements on datim Care & Treatment indicators
# TXNEW
#TXRTT
#TXML
# TXML(<3,3-5,6+)
# TRANSF OUT
# REFUSED/ STOPPED
# PMTCT ART
# CXCA_TX (actualização optional)
# TB ART (actualização optional)
</commit_message>
<xml_diff>
--- a/uploads/DHIS2 UPLOAD HISTORY.xlsx
+++ b/uploads/DHIS2 UPLOAD HISTORY.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1780,6 +1780,608 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2022-11-03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>MER HEALTH SYSTEM</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>EMR SITE</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>202209</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>FTLV9nOnAFC</t>
+        </is>
+      </c>
+      <c r="G34">
+        <v>200</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2022-11-03</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MER HEALTH SYSTEM</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>EMR SITE</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>202008</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>FTLV9nOnAFC</t>
+        </is>
+      </c>
+      <c r="G35">
+        <v>200</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2022-11-04</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MER HEALTH SYSTEM</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>EMR SITE</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>FTLV9nOnAFC</t>
+        </is>
+      </c>
+      <c r="G36">
+        <v>200</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2022-11-04</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MER HEALTH SYSTEM</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>EMR SITE</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>202009</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>FTLV9nOnAFC</t>
+        </is>
+      </c>
+      <c r="G37">
+        <v>200</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2022-11-08</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2022Q1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>KxezVOQ2TVR</t>
+        </is>
+      </c>
+      <c r="G38">
+        <v>200</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2022Q3</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>DoyPc35A7zI</t>
+        </is>
+      </c>
+      <c r="G39">
+        <v>200</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2022Q2</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>DoyPc35A7zI</t>
+        </is>
+      </c>
+      <c r="G40">
+        <v>200</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MER ATS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>DSD HTS TST</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2022Q1</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>DoyPc35A7zI</t>
+        </is>
+      </c>
+      <c r="G41">
+        <v>200</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2022Q1</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>XNYN71gD1ps</t>
+        </is>
+      </c>
+      <c r="G42">
+        <v>200</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2022Q4</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>aywqWn0Qkf8</t>
+        </is>
+      </c>
+      <c r="G43">
+        <v>200</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2022Q3</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>aywqWn0Qkf8</t>
+        </is>
+      </c>
+      <c r="G44">
+        <v>200</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2022-11-11</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>MER SMI</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>DSD PMTCT STAT</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2022Q3</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>aywqWn0Qkf8</t>
+        </is>
+      </c>
+      <c r="G45">
+        <v>200</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2022-11-11</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MER ATS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>DSD HTS TST</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2022Q3</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>aywqWn0Qkf8</t>
+        </is>
+      </c>
+      <c r="G46">
+        <v>200</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2022-11-11</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>DSD TX NEW</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2022Q3</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>kt468XD802Y</t>
+        </is>
+      </c>
+      <c r="G47">
+        <v>200</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Sucess</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>https://mail.ccsaude.org.mz:5455/api/33/dataValueSets</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>